<commit_message>
updated homework question list
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Joe Stanley\Joe's Documents\University of Idaho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC2103-3DB0-48B1-9492-614A77E9A7C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6FFE9C-D90A-4937-81C3-EECE15FA3373}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
   <si>
     <t>Vendor</t>
   </si>
@@ -587,9 +587,6 @@
     <t>14, 20, 21, 22, 23</t>
   </si>
   <si>
-    <t>4, 6, 30</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Com. Network: </t>
     </r>
@@ -609,6 +606,21 @@
   </si>
   <si>
     <t>8, 33</t>
+  </si>
+  <si>
+    <t>*Given test statement with ':=' instead of '='* What is wrong with this structured text statement?</t>
+  </si>
+  <si>
+    <t>What does POU stand for? What can a POU be?</t>
+  </si>
+  <si>
+    <t>Why shouldn't you call a program in PLC logic?</t>
+  </si>
+  <si>
+    <t>Why are wait() or while(1) statements not ideal for use in embedded (PLC) programming?</t>
+  </si>
+  <si>
+    <t>4, 6, 30, 34, 35, 36, 37</t>
   </si>
 </sst>
 </file>
@@ -742,9 +754,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -752,6 +761,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1092,13 +1104,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1255,7 +1267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1322,7 +1334,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -1777,7 +1789,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1819,128 +1831,128 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2056,10 +2068,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:B34"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2075,18 +2087,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2099,263 +2111,275 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
+      <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="15">
+      <c r="A17" s="14">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="15">
+      <c r="A18" s="14">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="12">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
+      <c r="A20" s="12">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="A21" s="12">
         <v>20</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
+      <c r="A22" s="12">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
+      <c r="A23" s="12">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
+      <c r="A24" s="12">
         <v>23</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="13">
+      <c r="A27" s="12">
         <v>26</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
+      <c r="A28" s="12">
         <v>27</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="A29" s="8">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+      <c r="A30" s="8">
         <v>29</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
+      <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>137</v>
+      <c r="B34" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
+      <c r="B35" s="10" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
+      <c r="B36" s="10" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="10">
         <v>36</v>
       </c>
+      <c r="B37" s="10" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="10">
         <v>37</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2396,11 +2420,6 @@
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with new question
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Joe Stanley\Joe's Documents\University of Idaho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Stanley\Google Drive\School\Industrial Controls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3EDA41-F41A-43B0-9CE8-70E80F73E0BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7361B0D-AEE6-44DD-903F-908C643E5F9E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="16900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Notes" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
   <si>
     <t>Vendor</t>
   </si>
@@ -629,12 +628,21 @@
   <si>
     <t>*Given motor rated current* Estimate the standard peak startup current for this motor.</t>
   </si>
+  <si>
+    <t>Generate AutomationDirect P2000 settings to perform a logical AND of two digital inputs and set an output.</t>
+  </si>
+  <si>
+    <t>PLC Project</t>
+  </si>
+  <si>
+    <t>40,</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -667,6 +675,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -744,7 +759,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -767,10 +782,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1094,35 +1115,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1145,7 +1166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1167,17 +1188,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1185,12 +1206,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1210,22 +1231,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1233,7 +1254,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1241,7 +1262,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1249,7 +1270,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -1274,19 +1295,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A6" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" customWidth="1"/>
-    <col min="3" max="3" width="53.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1300,7 +1321,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1311,7 +1332,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -1322,7 +1343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1333,7 +1354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1355,7 +1376,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6.1</v>
       </c>
@@ -1366,7 +1387,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6.2</v>
       </c>
@@ -1377,7 +1398,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1388,7 +1409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1399,7 +1420,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1439,17 +1460,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -1469,7 +1490,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1489,7 +1510,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1500,7 +1521,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1517,7 +1538,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1534,7 +1555,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1548,7 +1569,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1562,7 +1583,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1576,7 +1597,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1587,7 +1608,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1598,7 +1619,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1609,7 +1630,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1620,7 +1641,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1631,7 +1652,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1642,7 +1663,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1653,7 +1674,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1661,7 +1682,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1669,7 +1690,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1677,7 +1698,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1685,7 +1706,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1693,7 +1714,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1701,7 +1722,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1709,7 +1730,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1717,7 +1738,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1725,7 +1746,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1733,7 +1754,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1741,7 +1762,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1749,7 +1770,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1757,7 +1778,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1765,7 +1786,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1773,7 +1794,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1796,20 +1817,20 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -1823,7 +1844,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1837,7 +1858,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1851,7 +1872,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1865,7 +1886,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1879,77 +1900,77 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="11">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="12">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="B10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1957,108 +1978,117 @@
         <v>117</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2077,363 +2107,371 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView view="pageLayout" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="85.54296875" customWidth="1"/>
+    <col min="2" max="2" width="85.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="11">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="11">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="11">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="12">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="21" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="14">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="11">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="12">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="12">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="12">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="12">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="12">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="9">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="9">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="12">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="12">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="8">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="8">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="10">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="12">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="9">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
         <v>32</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="10">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="10">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="10">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="10">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="10">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="14">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="21">
         <v>38</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="21" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="14">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
         <v>39</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42">
+      <c r="B41" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43">
+      <c r="B42" s="17"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44">
+      <c r="B43" s="17"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45">
+      <c r="B44" s="17"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46">
+      <c r="B45" s="17"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
         <v>45</v>
       </c>
+      <c r="B46" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.78333333333333333" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2453,22 +2491,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.6328125" customWidth="1"/>
+    <col min="1" max="1" width="76.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
updated with new questions and better outline
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Stanley\Google Drive\School\Industrial Controls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Joe Stanley\Joe's Documents\University of Idaho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7361B0D-AEE6-44DD-903F-908C643E5F9E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4495A7E-553D-4878-929F-C98042E3C040}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="179">
   <si>
     <t>Vendor</t>
   </si>
@@ -389,27 +389,12 @@
     <t>Add'l Materials</t>
   </si>
   <si>
-    <t>HW</t>
-  </si>
-  <si>
     <t>Lect1</t>
   </si>
   <si>
-    <t>Sylabus/Intro-Defenitions</t>
-  </si>
-  <si>
     <t>Devices/Applications</t>
   </si>
   <si>
-    <t>HW0 Assigned</t>
-  </si>
-  <si>
-    <t>HW0 Due</t>
-  </si>
-  <si>
-    <t>HW1 Assigned</t>
-  </si>
-  <si>
     <t>Settings: Software</t>
   </si>
   <si>
@@ -434,9 +419,6 @@
     <t>TH</t>
   </si>
   <si>
-    <t>HW1 Due</t>
-  </si>
-  <si>
     <t>Data: SCADA Protocols (Mod/DNP/SEL)</t>
   </si>
   <si>
@@ -455,12 +437,6 @@
     <t>Settings: Intro/Software</t>
   </si>
   <si>
-    <t>HW2 Assigned</t>
-  </si>
-  <si>
-    <t>HW2 Due</t>
-  </si>
-  <si>
     <t>Vendor Websites</t>
   </si>
   <si>
@@ -536,30 +512,12 @@
     <t>Logic</t>
   </si>
   <si>
-    <t>1, 5, 28, 29</t>
-  </si>
-  <si>
-    <t>2, 15, 24, 25</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
     <t>Online DB</t>
   </si>
   <si>
-    <t>Relay Settings</t>
-  </si>
-  <si>
-    <t>RTAC Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">28, </t>
-  </si>
-  <si>
     <t>Web Quiz</t>
   </si>
   <si>
@@ -570,21 +528,6 @@
   </si>
   <si>
     <t>Match the SEL Protocol to the best-fit-application.</t>
-  </si>
-  <si>
-    <t>Networking (Serial)</t>
-  </si>
-  <si>
-    <t>Networking (Ethernet)</t>
-  </si>
-  <si>
-    <t>19, 26, 27, 31</t>
-  </si>
-  <si>
-    <t>7, 9, 10, 11, 12, 13, 18</t>
-  </si>
-  <si>
-    <t>14, 20, 21, 22, 23</t>
   </si>
   <si>
     <r>
@@ -629,20 +572,170 @@
     <t>*Given motor rated current* Estimate the standard peak startup current for this motor.</t>
   </si>
   <si>
-    <t>Generate AutomationDirect P2000 settings to perform a logical AND of two digital inputs and set an output.</t>
-  </si>
-  <si>
-    <t>PLC Project</t>
-  </si>
-  <si>
-    <t>40,</t>
+    <t>Assign</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>HW0</t>
+  </si>
+  <si>
+    <t>HW1</t>
+  </si>
+  <si>
+    <t>HW2</t>
+  </si>
+  <si>
+    <t>HW3</t>
+  </si>
+  <si>
+    <t>HW4</t>
+  </si>
+  <si>
+    <t>HW5</t>
+  </si>
+  <si>
+    <t>Sylabus/Devices/Applications</t>
+  </si>
+  <si>
+    <t>HW6</t>
+  </si>
+  <si>
+    <t>HW7</t>
+  </si>
+  <si>
+    <t>HW8</t>
+  </si>
+  <si>
+    <t>HW9</t>
+  </si>
+  <si>
+    <t>HW10</t>
+  </si>
+  <si>
+    <t>1, 5, 28</t>
+  </si>
+  <si>
+    <t>RTAC Project, PLC Project</t>
+  </si>
+  <si>
+    <t>29, 40</t>
+  </si>
+  <si>
+    <t>Web Quiz/File Submission</t>
+  </si>
+  <si>
+    <t>Networking (Serial/Ethernet)</t>
+  </si>
+  <si>
+    <t>Generate AutomationDirect P2000 settings for the *described* device.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Programming: Additional Material</t>
+  </si>
+  <si>
+    <t>Motors: Line Connected Starting</t>
+  </si>
+  <si>
+    <t>electricpy</t>
+  </si>
+  <si>
+    <t>*Given Wireshark Screenshot* Based on the Wireshark capture pictured here, what protocol is being used?</t>
+  </si>
+  <si>
+    <t>14, 19, 20, 21, 22, 23, 26, 27, 31, 41</t>
+  </si>
+  <si>
+    <t>IEC-61850 Cheat Sheet</t>
+  </si>
+  <si>
+    <t>Net Port Cheat Sheet</t>
+  </si>
+  <si>
+    <t>Motors: Variable Frequency Drives</t>
+  </si>
+  <si>
+    <t>Motors: Protection Basics</t>
+  </si>
+  <si>
+    <t>Trending: Data Aggregation Basics</t>
+  </si>
+  <si>
+    <t>Trending: Data Storage/Transport</t>
+  </si>
+  <si>
+    <t>Metering: KYZ Pulse Metering</t>
+  </si>
+  <si>
+    <t>Metering: Load Forecasting</t>
+  </si>
+  <si>
+    <t>HMI: Basics</t>
+  </si>
+  <si>
+    <t>Motors and Encoders</t>
+  </si>
+  <si>
+    <t>Are startup capacitors required for 3-phs motors? Are run capacitors required for 3-phs motors?</t>
+  </si>
+  <si>
+    <t>3, 16, 17, 38, 39, 42</t>
+  </si>
+  <si>
+    <t>*Given metering dataset (samples)* Which metering interval setting would accrue the most kWh? The least?</t>
+  </si>
+  <si>
+    <t>7, 9, 10, 11, 12, 18</t>
+  </si>
+  <si>
+    <t>Metering</t>
+  </si>
+  <si>
+    <t>13, 43</t>
+  </si>
+  <si>
+    <t>*Given RTAC and P2000 projects* Configure these projects to record *dataset* in a CSV format.</t>
+  </si>
+  <si>
+    <t>Trending and Data Aggregation</t>
+  </si>
+  <si>
+    <t>Exam 1 OR Project 1 Due</t>
+  </si>
+  <si>
+    <t>Exam 2 OR Project 2 Due</t>
+  </si>
+  <si>
+    <t>You need to control a relay contact in a remote IED, you're using DNP for coms, do you use a Digital-Input or -Output?</t>
+  </si>
+  <si>
+    <t>2, 15, 24, 25, 46</t>
+  </si>
+  <si>
+    <t>Match the RAID number to its best fit description.</t>
+  </si>
+  <si>
+    <t>*Describe application of particular RAID arrangement* Which RAID arrangement would best fit this application?</t>
+  </si>
+  <si>
+    <t>44, 45, 47</t>
+  </si>
+  <si>
+    <t>232/485 Pinout Cheat Sheet</t>
+  </si>
+  <si>
+    <t>Semester Review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,8 +779,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,6 +834,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -759,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -782,9 +911,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -792,6 +918,16 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -802,6 +938,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FFCCFF99"/>
       <color rgb="FFE2A5F3"/>
     </mruColors>
   </colors>
@@ -1115,35 +1253,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1166,7 +1304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1180,7 +1318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1188,17 +1326,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1206,12 +1344,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1231,22 +1369,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1254,7 +1392,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1262,7 +1400,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1270,7 +1408,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -1296,18 +1434,18 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1321,7 +1459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1332,7 +1470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -1343,7 +1481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1354,7 +1492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1362,10 +1500,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1376,7 +1514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6.1</v>
       </c>
@@ -1387,7 +1525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6.2</v>
       </c>
@@ -1398,7 +1536,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1409,7 +1547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1420,7 +1558,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1428,10 +1566,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1439,7 +1577,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1454,23 +1592,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1197D6-A180-457B-9464-A598275B3BD9}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -1484,325 +1623,440 @@
         <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>74</v>
+        <v>85</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" t="s">
         <v>78</v>
       </c>
-      <c r="E7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
         <v>77</v>
       </c>
-      <c r="F12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="F16" t="s">
+      <c r="B16" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
+      <c r="B17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="F18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="F19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="F20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="F21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="F22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="F25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="F26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="F28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="F29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="F30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="F31" t="s">
-        <v>83</v>
+      <c r="B31" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <headerFooter>
@@ -1817,20 +2071,20 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -1838,259 +2092,259 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="B3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B4" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="D9" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="B10" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="B11" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="B12" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2105,373 +2359,573 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="85.5703125" customWidth="1"/>
+    <col min="2" max="2" width="85.5546875" customWidth="1"/>
+    <col min="3" max="3" width="3.21875" customWidth="1"/>
+    <col min="4" max="4" width="86.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="C2" s="15">
+        <v>46</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="C3" s="25">
+        <v>47</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="C4" s="16">
+        <v>48</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="C5" s="16">
+        <v>49</v>
+      </c>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="C6" s="16">
+        <v>50</v>
+      </c>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="C7" s="16">
+        <v>51</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="16">
+        <v>52</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="16">
+        <v>53</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="16">
+        <v>54</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="16">
+        <v>55</v>
+      </c>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="16">
+        <v>56</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
+        <v>12</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="16">
+        <v>57</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="23">
+        <v>13</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="16">
+        <v>58</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="16">
+        <v>59</v>
+      </c>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="16">
+        <v>60</v>
+      </c>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="20">
+        <v>16</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="16">
+        <v>61</v>
+      </c>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="20">
+        <v>17</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="16">
+        <v>62</v>
+      </c>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>18</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="16">
+        <v>63</v>
+      </c>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>19</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="16">
+        <v>64</v>
+      </c>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="19">
+        <v>20</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="16">
+        <v>65</v>
+      </c>
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="19">
+        <v>21</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="16">
+        <v>66</v>
+      </c>
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="16">
+        <v>67</v>
+      </c>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="19">
+        <v>23</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="16">
+        <v>68</v>
+      </c>
+      <c r="D24" s="16"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>8</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <v>9</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>10</v>
-      </c>
-      <c r="B11" s="19" t="s">
+      <c r="C25" s="16">
+        <v>69</v>
+      </c>
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="16">
+        <v>70</v>
+      </c>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="19">
+        <v>26</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>11</v>
-      </c>
-      <c r="B12" s="19" t="s">
+      <c r="C27" s="16">
+        <v>71</v>
+      </c>
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="19">
+        <v>27</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>12</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>13</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
-        <v>14</v>
-      </c>
-      <c r="B15" s="20" t="s">
+      <c r="C28" s="16">
+        <v>72</v>
+      </c>
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>28</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="C29" s="16">
+        <v>73</v>
+      </c>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>16</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
-        <v>17</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>20</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
-        <v>21</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
-        <v>22</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>23</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
-        <v>24</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
-        <v>25</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
-        <v>26</v>
-      </c>
-      <c r="B27" s="20" t="s">
+      <c r="C30" s="16">
+        <v>74</v>
+      </c>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="17">
+        <v>30</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
-        <v>27</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
-        <v>28</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
-        <v>29</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="18">
-        <v>30</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
+      <c r="C31" s="16">
+        <v>75</v>
+      </c>
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="19">
         <v>31</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
+      <c r="B32" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="16">
+        <v>76</v>
+      </c>
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
         <v>32</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="18">
+      <c r="B33" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="16">
+        <v>77</v>
+      </c>
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="17">
         <v>33</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
+      <c r="B34" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="16">
+        <v>78</v>
+      </c>
+      <c r="D34" s="16"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="17">
         <v>34</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="18">
+      <c r="B35" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="16">
+        <v>79</v>
+      </c>
+      <c r="D35" s="16"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="17">
         <v>35</v>
       </c>
-      <c r="B36" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="18">
+      <c r="B36" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="16">
+        <v>80</v>
+      </c>
+      <c r="D36" s="16"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="17">
         <v>36</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="18">
+      <c r="B37" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="16">
+        <v>81</v>
+      </c>
+      <c r="D37" s="16"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="17">
         <v>37</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="21">
+      <c r="B38" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="16">
+        <v>82</v>
+      </c>
+      <c r="D38" s="16"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="20">
         <v>38</v>
       </c>
-      <c r="B39" s="21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="21">
+      <c r="B39" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="16">
+        <v>83</v>
+      </c>
+      <c r="D39" s="16"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="20">
         <v>39</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
+      <c r="B40" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="16">
+        <v>84</v>
+      </c>
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
         <v>40</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="C41" s="16">
+        <v>85</v>
+      </c>
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="19">
         <v>41</v>
       </c>
-      <c r="B42" s="17"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="B42" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="16">
+        <v>86</v>
+      </c>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="20">
         <v>42</v>
       </c>
-      <c r="B43" s="17"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+      <c r="B43" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="16">
+        <v>87</v>
+      </c>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="23">
         <v>43</v>
       </c>
-      <c r="B44" s="17"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+      <c r="B44" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="16">
+        <v>88</v>
+      </c>
+      <c r="D44" s="16"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="25">
         <v>44</v>
       </c>
-      <c r="B45" s="17"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+      <c r="B45" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="16">
+        <v>89</v>
+      </c>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="25">
         <v>45</v>
       </c>
-      <c r="B46" s="17"/>
+      <c r="B46" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="16">
+        <v>90</v>
+      </c>
+      <c r="D46" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.78333333333333333" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2491,22 +2945,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76.5703125" customWidth="1"/>
+    <col min="1" max="1" width="76.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
added a few new questions
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\Desktop\UI_CONTROLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9F13B1-0C81-46F1-82B7-885DDA27CD16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2698F6A-C222-44A1-AF81-08256A7EFD65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="204">
   <si>
     <t>Vendor</t>
   </si>
@@ -729,6 +729,81 @@
   </si>
   <si>
     <t>Semester Review</t>
+  </si>
+  <si>
+    <t>Why wouldn't standard digital outputs be a good idea for controlling a stepper or servo motor?</t>
+  </si>
+  <si>
+    <t>Difference wouldn't standard digital outputs be q good idebetween controlling q stepper AcSELerator servo and?</t>
+  </si>
+  <si>
+    <t>Primary wouldn't standard digital outputs be " good idelanguages controlling " stepper 61131 servo available?</t>
+  </si>
+  <si>
+    <t>In wouldn't standard digital outputs be o good ideST a controlling o stepper an servo a?</t>
+  </si>
+  <si>
+    <t>Standard wouldn't standard digital outputs be i good ideinput mV controlling i stepper inputs servo sensors?</t>
+  </si>
+  <si>
+    <t>Rtd wouldn't standard digital outputs be c good idesensor could controlling c stepper Couple servo be?</t>
+  </si>
+  <si>
+    <t>Sys wouldn't standard digital outputs be p good idegiven and controlling p stepper roll servo pulse?</t>
+  </si>
+  <si>
+    <t>Accuracy wouldn't standard digital outputs be a good idefor an controlling a stepper the servo analog?</t>
+  </si>
+  <si>
+    <t>Two wouldn't standard digital outputs be a good idediscrete known controlling a stepper IPv servo commonly?</t>
+  </si>
+  <si>
+    <t>Stand wouldn't standard digital outputs be c good idefor controlling c stepper Routing servo Inter?</t>
+  </si>
+  <si>
+    <t>Re wouldn't standard digital outputs be a good idewritten controlling a stepper notation servo using?</t>
+  </si>
+  <si>
+    <t>Difference wouldn't standard digital outputs be a good idebetween network controlling a stepper switch servo a?</t>
+  </si>
+  <si>
+    <t>Protocol wouldn't standard digital outputs be m good ideModbus similar controlling m stepper IEC servo most?</t>
+  </si>
+  <si>
+    <t>Settings wouldn't standard digital outputs be s good ideand controlling s stepper as servo as?</t>
+  </si>
+  <si>
+    <t>What is the purpose of termination resistors in EIA485?</t>
+  </si>
+  <si>
+    <t>Wndamental is Calculate purpose of termination resistfors -p EIA785?</t>
+  </si>
+  <si>
+    <t>W is type purpose of termination resistands ol EIA1185?</t>
+  </si>
+  <si>
+    <t>What is and purpose of termination resistinputs fi EIA1285?</t>
+  </si>
+  <si>
+    <t>Wonnect to is to purpose of termination resistYou'res ra EIA1485?</t>
+  </si>
+  <si>
+    <t>Wom is developing purpose of termination resistInfos re EIA1585?</t>
+  </si>
+  <si>
+    <t>Wo is Given purpose of termination resistfroms ha EIA1685?</t>
+  </si>
+  <si>
+    <t>W wa is encoder purpose of termination resistchainss se EIA1785?</t>
+  </si>
+  <si>
+    <t>Wm is the purpose of termination resistdiagramss ir EIA1985?</t>
+  </si>
+  <si>
+    <t>W function is the purpose of termination resistValuess Sc EIA2485?</t>
+  </si>
+  <si>
+    <t>Why wouldn't EIA232 be a good choice for communications over long distances?</t>
   </si>
 </sst>
 </file>
@@ -2361,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2421,7 +2496,9 @@
       <c r="C4" s="16">
         <v>48</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="17">
@@ -2433,7 +2510,9 @@
       <c r="C5" s="16">
         <v>49</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
@@ -2445,7 +2524,9 @@
       <c r="C6" s="16">
         <v>50</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="17">

</xml_diff>

<commit_message>
started with presentation 1
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\Desktop\UI_CONTROLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2698F6A-C222-44A1-AF81-08256A7EFD65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A7D7F-0A77-4EFD-8CCF-51831523C12E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="183">
   <si>
     <t>Vendor</t>
   </si>
@@ -734,76 +734,13 @@
     <t>Why wouldn't standard digital outputs be a good idea for controlling a stepper or servo motor?</t>
   </si>
   <si>
-    <t>Difference wouldn't standard digital outputs be q good idebetween controlling q stepper AcSELerator servo and?</t>
-  </si>
-  <si>
-    <t>Primary wouldn't standard digital outputs be " good idelanguages controlling " stepper 61131 servo available?</t>
-  </si>
-  <si>
-    <t>In wouldn't standard digital outputs be o good ideST a controlling o stepper an servo a?</t>
-  </si>
-  <si>
-    <t>Standard wouldn't standard digital outputs be i good ideinput mV controlling i stepper inputs servo sensors?</t>
-  </si>
-  <si>
-    <t>Rtd wouldn't standard digital outputs be c good idesensor could controlling c stepper Couple servo be?</t>
-  </si>
-  <si>
-    <t>Sys wouldn't standard digital outputs be p good idegiven and controlling p stepper roll servo pulse?</t>
-  </si>
-  <si>
-    <t>Accuracy wouldn't standard digital outputs be a good idefor an controlling a stepper the servo analog?</t>
-  </si>
-  <si>
-    <t>Two wouldn't standard digital outputs be a good idediscrete known controlling a stepper IPv servo commonly?</t>
-  </si>
-  <si>
-    <t>Stand wouldn't standard digital outputs be c good idefor controlling c stepper Routing servo Inter?</t>
-  </si>
-  <si>
-    <t>Re wouldn't standard digital outputs be a good idewritten controlling a stepper notation servo using?</t>
-  </si>
-  <si>
-    <t>Difference wouldn't standard digital outputs be a good idebetween network controlling a stepper switch servo a?</t>
-  </si>
-  <si>
-    <t>Protocol wouldn't standard digital outputs be m good ideModbus similar controlling m stepper IEC servo most?</t>
-  </si>
-  <si>
-    <t>Settings wouldn't standard digital outputs be s good ideand controlling s stepper as servo as?</t>
-  </si>
-  <si>
     <t>What is the purpose of termination resistors in EIA485?</t>
   </si>
   <si>
-    <t>Wndamental is Calculate purpose of termination resistfors -p EIA785?</t>
-  </si>
-  <si>
-    <t>W is type purpose of termination resistands ol EIA1185?</t>
-  </si>
-  <si>
-    <t>What is and purpose of termination resistinputs fi EIA1285?</t>
-  </si>
-  <si>
-    <t>Wonnect to is to purpose of termination resistYou'res ra EIA1485?</t>
-  </si>
-  <si>
-    <t>Wom is developing purpose of termination resistInfos re EIA1585?</t>
-  </si>
-  <si>
-    <t>Wo is Given purpose of termination resistfroms ha EIA1685?</t>
-  </si>
-  <si>
-    <t>W wa is encoder purpose of termination resistchainss se EIA1785?</t>
-  </si>
-  <si>
-    <t>Wm is the purpose of termination resistdiagramss ir EIA1985?</t>
-  </si>
-  <si>
-    <t>W function is the purpose of termination resistValuess Sc EIA2485?</t>
-  </si>
-  <si>
     <t>Why wouldn't EIA232 be a good choice for communications over long distances?</t>
+  </si>
+  <si>
+    <t>SEL Terminal Cheet Sheet</t>
   </si>
 </sst>
 </file>
@@ -1669,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1197D6-A180-457B-9464-A598275B3BD9}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1767,6 +1704,9 @@
       </c>
       <c r="B5" t="s">
         <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>182</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>130</v>
@@ -2436,7 +2376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2511,7 +2451,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -2525,7 +2465,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated pres1 and added cheat sheets
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\Desktop\UI_CONTROLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Joe Stanley\Joe's Documents\University of Idaho\Industrial Controls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A7D7F-0A77-4EFD-8CCF-51831523C12E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B88EF26-4A9C-46B4-A7F1-DF79EE1C3942}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="184">
   <si>
     <t>Vendor</t>
   </si>
@@ -407,9 +407,6 @@
     <t>Data: Inputs/Outputs, RTD/TC</t>
   </si>
   <si>
-    <t>Sylabus, Cheat Sheet</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -741,6 +738,12 @@
   </si>
   <si>
     <t>SEL Terminal Cheet Sheet</t>
+  </si>
+  <si>
+    <t>Metering: Energy Packets</t>
+  </si>
+  <si>
+    <t>Sylabus, TLA/FLA Cheat Sheet</t>
   </si>
 </sst>
 </file>
@@ -1269,16 +1272,16 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1338,17 +1341,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1356,12 +1359,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1381,22 +1384,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -1449,15 +1452,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" customWidth="1"/>
-    <col min="3" max="3" width="53.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1504,7 +1507,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1512,10 +1515,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6.1</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6.2</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1607,21 +1610,21 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" customWidth="1"/>
-    <col min="7" max="7" width="4.54296875" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -1635,36 +1638,36 @@
         <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1672,33 +1675,33 @@
         <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
         <v>84</v>
       </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1706,19 +1709,19 @@
         <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1726,19 +1729,19 @@
         <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1746,106 +1749,106 @@
         <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1853,221 +1856,224 @@
         <v>72</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
       <c r="G28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2089,17 +2095,17 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" customWidth="1"/>
-    <col min="3" max="3" width="33.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -2107,257 +2113,257 @@
         <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="D4" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>8</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
         <v>9</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>167</v>
-      </c>
       <c r="D12" s="23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2380,15 +2386,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="85.54296875" customWidth="1"/>
-    <col min="3" max="3" width="3.1796875" customWidth="1"/>
-    <col min="4" max="4" width="86.08984375" customWidth="1"/>
+    <col min="2" max="2" width="85.5546875" customWidth="1"/>
+    <col min="3" max="3" width="3.21875" customWidth="1"/>
+    <col min="4" max="4" width="86.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>38</v>
@@ -2398,7 +2404,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2409,10 +2415,10 @@
         <v>46</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2423,10 +2429,10 @@
         <v>47</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -2437,10 +2443,10 @@
         <v>48</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -2451,10 +2457,10 @@
         <v>49</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -2465,10 +2471,10 @@
         <v>50</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -2480,31 +2486,31 @@
       </c>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="16">
         <v>52</v>
       </c>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="16">
         <v>53</v>
       </c>
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -2516,31 +2522,31 @@
       </c>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="16">
         <v>55</v>
       </c>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="16">
         <v>56</v>
       </c>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -2552,55 +2558,55 @@
       </c>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>13</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="16">
         <v>58</v>
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="16">
         <v>59</v>
       </c>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="16">
         <v>60</v>
       </c>
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="16">
         <v>61</v>
       </c>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>17</v>
       </c>
@@ -2612,31 +2618,31 @@
       </c>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="16">
         <v>63</v>
       </c>
       <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="16">
         <v>64</v>
       </c>
       <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -2648,7 +2654,7 @@
       </c>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -2660,7 +2666,7 @@
       </c>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -2672,7 +2678,7 @@
       </c>
       <c r="D23" s="16"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -2684,19 +2690,19 @@
       </c>
       <c r="D24" s="16"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="16">
         <v>69</v>
       </c>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -2708,240 +2714,240 @@
       </c>
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="16">
         <v>71</v>
       </c>
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="16">
         <v>72</v>
       </c>
       <c r="D28" s="16"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="16">
         <v>73</v>
       </c>
       <c r="D29" s="16"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
         <v>29</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="16">
         <v>74</v>
       </c>
       <c r="D30" s="16"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" s="16">
         <v>75</v>
       </c>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C32" s="16">
         <v>76</v>
       </c>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" s="16">
         <v>77</v>
       </c>
       <c r="D33" s="16"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="17">
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" s="16">
         <v>78</v>
       </c>
       <c r="D34" s="16"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
         <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="16">
         <v>79</v>
       </c>
       <c r="D35" s="16"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" s="16">
         <v>80</v>
       </c>
       <c r="D36" s="16"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C37" s="16">
         <v>81</v>
       </c>
       <c r="D37" s="16"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="17">
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C38" s="16">
         <v>82</v>
       </c>
       <c r="D38" s="16"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="20">
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C39" s="16">
         <v>83</v>
       </c>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="20">
         <v>39</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C40" s="16">
         <v>84</v>
       </c>
       <c r="D40" s="16"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
         <v>40</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="16">
         <v>85</v>
       </c>
       <c r="D41" s="16"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>41</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" s="16">
         <v>86</v>
       </c>
       <c r="D42" s="16"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="20">
         <v>42</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C43" s="16">
         <v>87</v>
       </c>
       <c r="D43" s="16"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="22">
         <v>43</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" s="16">
         <v>88</v>
       </c>
       <c r="D44" s="16"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="24">
         <v>44</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C45" s="16">
         <v>89</v>
       </c>
       <c r="D45" s="16"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="24">
         <v>45</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C46" s="16">
         <v>90</v>
@@ -2966,22 +2972,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76.54296875" customWidth="1"/>
+    <col min="1" max="1" width="76.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
added question and acronyms
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\Desktop\UI_CONTROLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A973545A-BA73-4F25-B5BC-304E3DCD6899}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A78BEAE-0E32-4DCE-8693-34B36D920D67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="185">
   <si>
     <t>Vendor</t>
   </si>
@@ -744,6 +744,9 @@
   </si>
   <si>
     <t>Sylabus, TLA/FLA Cheat Sheet</t>
+  </si>
+  <si>
+    <t>*Given two datasets* Apply a Cosine filter, using a instantaneous trip setting of x, how long before trip setting pickup?</t>
   </si>
 </sst>
 </file>
@@ -1609,7 +1612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1197D6-A180-457B-9464-A598275B3BD9}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2382,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2484,7 +2487,9 @@
       <c r="C7" s="16">
         <v>51</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="18">

</xml_diff>

<commit_message>
updated tla/fla and added placeholder documents for SEL and DNP protocol cheat sheets
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\Desktop\UI_CONTROLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\OneDrive - Schweitzer Engineering Laboratories\Customer Projects\University of Idaho\Industrial Controls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A78BEAE-0E32-4DCE-8693-34B36D920D67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{7A78BEAE-0E32-4DCE-8693-34B36D920D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FC75EB3-2D6D-4D24-AA8B-AFBD66EA8672}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="195">
   <si>
     <t>Vendor</t>
   </si>
@@ -548,9 +548,6 @@
     <t>8, 33</t>
   </si>
   <si>
-    <t>*Given test statement with ':=' instead of '='* What is wrong with this structured text statement?</t>
-  </si>
-  <si>
     <t>What does POU stand for? What can a POU be?</t>
   </si>
   <si>
@@ -747,6 +744,39 @@
   </si>
   <si>
     <t>*Given two datasets* Apply a Cosine filter, using a instantaneous trip setting of x, how long before trip setting pickup?</t>
+  </si>
+  <si>
+    <t>*Given test statement with ':=' instead of '='* What is wrong with this IEC-61131 structured text statement?</t>
+  </si>
+  <si>
+    <t>Will  all data be collected in a class 1 poll in DNP?</t>
+  </si>
+  <si>
+    <t>What event data is typically assocaited with a class 0 poll? Class 1? Class 2? Class 3?</t>
+  </si>
+  <si>
+    <t>Suggest two reasons that analog values reported by DNP is evaluated as "0" when it is actually measuring a small value.</t>
+  </si>
+  <si>
+    <t>Are Telnet communications encrypted?</t>
+  </si>
+  <si>
+    <t>Can Modbus RTU be used over Ethernet?</t>
+  </si>
+  <si>
+    <t>Is Modbus TCP equivalent to Modbus RTU over Ethernet?</t>
+  </si>
+  <si>
+    <t>Can Modbus input registers be written to from a client/master?</t>
+  </si>
+  <si>
+    <t>Which terms are essentially equivalent: (Master/Slave/Client/Server)?</t>
+  </si>
+  <si>
+    <t>In most vendor implementations, are Modbus maps configurable?</t>
+  </si>
+  <si>
+    <t>In most vendor implementations, are DNP maps configurable?</t>
   </si>
 </sst>
 </file>
@@ -1641,10 +1671,10 @@
         <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>75</v>
@@ -1655,16 +1685,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G2" t="s">
         <v>76</v>
@@ -1695,10 +1725,10 @@
         <v>84</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" t="s">
         <v>76</v>
@@ -1712,13 +1742,13 @@
         <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" t="s">
         <v>77</v>
@@ -1732,13 +1762,13 @@
         <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" t="s">
         <v>76</v>
@@ -1763,13 +1793,13 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" t="s">
         <v>76</v>
@@ -1783,7 +1813,7 @@
         <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G9" t="s">
         <v>77</v>
@@ -1797,13 +1827,13 @@
         <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G10" t="s">
         <v>76</v>
@@ -1836,16 +1866,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G13" t="s">
         <v>77</v>
@@ -1859,7 +1889,7 @@
         <v>72</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G14" t="s">
         <v>76</v>
@@ -1873,7 +1903,7 @@
         <v>80</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
         <v>77</v>
@@ -1906,10 +1936,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G18" t="s">
         <v>76</v>
@@ -1920,13 +1950,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
         <v>77</v>
@@ -1937,7 +1967,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G20" t="s">
         <v>76</v>
@@ -1948,7 +1978,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G21" t="s">
         <v>77</v>
@@ -1959,16 +1989,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G22" t="s">
         <v>76</v>
@@ -1979,10 +2009,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G23" t="s">
         <v>77</v>
@@ -1993,7 +2023,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G24" t="s">
         <v>76</v>
@@ -2004,13 +2034,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G25" t="s">
         <v>77</v>
@@ -2021,7 +2051,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G26" t="s">
         <v>76</v>
@@ -2032,10 +2062,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G27" t="s">
         <v>77</v>
@@ -2046,7 +2076,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G28" t="s">
         <v>76</v>
@@ -2073,7 +2103,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G31" t="s">
         <v>77</v>
@@ -2144,10 +2174,10 @@
         <v>105</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2155,10 +2185,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>112</v>
@@ -2172,7 +2202,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>111</v>
@@ -2186,7 +2216,7 @@
         <v>107</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>111</v>
@@ -2197,10 +2227,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>111</v>
@@ -2214,7 +2244,7 @@
         <v>108</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>111</v>
@@ -2239,10 +2269,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>111</v>
@@ -2253,13 +2283,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2267,10 +2297,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>165</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>166</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>111</v>
@@ -2385,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2418,7 +2448,7 @@
         <v>46</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2432,7 +2462,7 @@
         <v>47</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2446,7 +2476,7 @@
         <v>48</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2460,7 +2490,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -2474,7 +2504,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2488,7 +2518,7 @@
         <v>51</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2501,7 +2531,9 @@
       <c r="C8" s="16">
         <v>52</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="16" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="17">
@@ -2513,7 +2545,9 @@
       <c r="C9" s="16">
         <v>53</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
@@ -2525,7 +2559,9 @@
       <c r="C10" s="16">
         <v>54</v>
       </c>
-      <c r="D10" s="16"/>
+      <c r="D10" s="16" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
@@ -2537,7 +2573,9 @@
       <c r="C11" s="16">
         <v>55</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="16" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
@@ -2549,7 +2587,9 @@
       <c r="C12" s="16">
         <v>56</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
@@ -2561,7 +2601,9 @@
       <c r="C13" s="16">
         <v>57</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
@@ -2573,7 +2615,9 @@
       <c r="C14" s="16">
         <v>58</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="16" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="19">
@@ -2585,7 +2629,9 @@
       <c r="C15" s="16">
         <v>59</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="16" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
@@ -2597,7 +2643,9 @@
       <c r="C16" s="16">
         <v>60</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="16" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="20">
@@ -2609,7 +2657,9 @@
       <c r="C17" s="16">
         <v>61</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="16" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="20">
@@ -2820,7 +2870,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>118</v>
+        <v>184</v>
       </c>
       <c r="C35" s="16">
         <v>79</v>
@@ -2832,7 +2882,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="16">
         <v>80</v>
@@ -2844,7 +2894,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C37" s="16">
         <v>81</v>
@@ -2856,7 +2906,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C38" s="16">
         <v>82</v>
@@ -2868,7 +2918,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" s="16">
         <v>83</v>
@@ -2880,7 +2930,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" s="16">
         <v>84</v>
@@ -2892,7 +2942,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C41" s="16">
         <v>85</v>
@@ -2904,7 +2954,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="16">
         <v>86</v>
@@ -2916,7 +2966,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C43" s="16">
         <v>87</v>
@@ -2928,7 +2978,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" s="16">
         <v>88</v>
@@ -2940,7 +2990,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C45" s="16">
         <v>89</v>
@@ -2952,7 +3002,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C46" s="16">
         <v>90</v>

</xml_diff>

<commit_message>
updated deadband example script and created acrtac screenshot script
</commit_message>
<xml_diff>
--- a/Industrial Controls Notes.xlsx
+++ b/Industrial Controls Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joestan\OneDrive - Schweitzer Engineering Laboratories\Customer Projects\University of Idaho\Industrial Controls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{7A78BEAE-0E32-4DCE-8693-34B36D920D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FC75EB3-2D6D-4D24-AA8B-AFBD66EA8672}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{7A78BEAE-0E32-4DCE-8693-34B36D920D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FD7C781-BD5E-4CD6-B1E2-039E40185504}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="207">
   <si>
     <t>Vendor</t>
   </si>
@@ -777,6 +777,42 @@
   </si>
   <si>
     <t>In most vendor implementations, are DNP maps configurable?</t>
+  </si>
+  <si>
+    <t>*Given network connection diagram* Which device is the server? Which device is the client?</t>
+  </si>
+  <si>
+    <t>Select all attributes that are provided in an IRIG-B-002 communication. (day, month, hour, minute, second - no year!)</t>
+  </si>
+  <si>
+    <t>*Given engineering units scaling information* If the analog input measures 7.56mA, what will the output value be?</t>
+  </si>
+  <si>
+    <t>*Given analog input resolution value and sensory input range* Evaluate the sensory resolution for the analog input.</t>
+  </si>
+  <si>
+    <t>*Given motor's power in watts* Evaluate the horsepower rating of the specified motor.</t>
+  </si>
+  <si>
+    <t>*Given pulse count resolution of rotary encoder* What is the smallest angular unit that this rotary encoder will record?</t>
+  </si>
+  <si>
+    <t>What does MSB indicate? How about LSB?</t>
+  </si>
+  <si>
+    <t>What level of current should motor contactors be rated for?</t>
+  </si>
+  <si>
+    <t>What sort of cable (null-modem/straight-through) should be used for communications between an RTAC and relay?</t>
+  </si>
+  <si>
+    <t>*Given voltage scaling information -PTR/scale/input-level* What should a technician expect to see as an output voltage?</t>
+  </si>
+  <si>
+    <t>Suggest reasons why there are both AC and DC contact ratings for switches and relay contacts.</t>
+  </si>
+  <si>
+    <t>*Given a link-budget diagram* What will the receive power be given an input power (some dB value)?</t>
   </si>
 </sst>
 </file>
@@ -2415,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A23" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2671,7 +2707,9 @@
       <c r="C18" s="16">
         <v>62</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
@@ -2683,7 +2721,9 @@
       <c r="C19" s="16">
         <v>63</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="16" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="19">
@@ -2695,7 +2735,9 @@
       <c r="C20" s="16">
         <v>64</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="16" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="19">
@@ -2707,7 +2749,9 @@
       <c r="C21" s="16">
         <v>65</v>
       </c>
-      <c r="D21" s="16"/>
+      <c r="D21" s="16" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="19">
@@ -2719,7 +2763,9 @@
       <c r="C22" s="16">
         <v>66</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="19">
@@ -2731,7 +2777,9 @@
       <c r="C23" s="16">
         <v>67</v>
       </c>
-      <c r="D23" s="16"/>
+      <c r="D23" s="16" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="19">
@@ -2743,7 +2791,9 @@
       <c r="C24" s="16">
         <v>68</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="16" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
@@ -2755,7 +2805,9 @@
       <c r="C25" s="16">
         <v>69</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="16" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
@@ -2767,7 +2819,9 @@
       <c r="C26" s="16">
         <v>70</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="16" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="19">
@@ -2779,7 +2833,9 @@
       <c r="C27" s="16">
         <v>71</v>
       </c>
-      <c r="D27" s="16"/>
+      <c r="D27" s="16" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="19">
@@ -2791,7 +2847,9 @@
       <c r="C28" s="16">
         <v>72</v>
       </c>
-      <c r="D28" s="16"/>
+      <c r="D28" s="16" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
@@ -2803,7 +2861,9 @@
       <c r="C29" s="16">
         <v>73</v>
       </c>
-      <c r="D29" s="16"/>
+      <c r="D29" s="16" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="14">

</xml_diff>